<commit_message>
added element to be clicked and a click script for javascript page
</commit_message>
<xml_diff>
--- a/Autostockin/stockin49.xlsx
+++ b/Autostockin/stockin49.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Autostockin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD9C547-3F93-4CAC-BB6A-E8C78B811B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF93799-9DC0-4959-B503-41C6C33D3F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="3180" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="595">
   <si>
     <t>+186-1517</t>
   </si>
@@ -1324,6 +1324,498 @@
   </si>
   <si>
     <t>23800</t>
+  </si>
+  <si>
+    <t>+3620-796</t>
+  </si>
+  <si>
+    <t>+593-1194</t>
+  </si>
+  <si>
+    <t>+6448-633</t>
+  </si>
+  <si>
+    <t>+17294-220</t>
+  </si>
+  <si>
+    <t>+1333-594</t>
+  </si>
+  <si>
+    <t>+17297-220</t>
+  </si>
+  <si>
+    <t>+21998-106</t>
+  </si>
+  <si>
+    <t>+22046-182</t>
+  </si>
+  <si>
+    <t>+19466-646</t>
+  </si>
+  <si>
+    <t>+552-1087</t>
+  </si>
+  <si>
+    <t>+173035-33</t>
+  </si>
+  <si>
+    <t>+754-1480</t>
+  </si>
+  <si>
+    <t>+17292-220</t>
+  </si>
+  <si>
+    <t>+814-1445</t>
+  </si>
+  <si>
+    <t>+817-1445</t>
+  </si>
+  <si>
+    <t>+813-1445</t>
+  </si>
+  <si>
+    <t>+17290-220</t>
+  </si>
+  <si>
+    <t>+816-1445</t>
+  </si>
+  <si>
+    <t>+173032-33</t>
+  </si>
+  <si>
+    <t>+173031-33</t>
+  </si>
+  <si>
+    <t>+22056-182</t>
+  </si>
+  <si>
+    <t>+788-1402</t>
+  </si>
+  <si>
+    <t>+15015-335</t>
+  </si>
+  <si>
+    <t>+17291-220</t>
+  </si>
+  <si>
+    <t>+17295-220</t>
+  </si>
+  <si>
+    <t>+17296-220</t>
+  </si>
+  <si>
+    <t>+12542-314</t>
+  </si>
+  <si>
+    <t>+811-1445</t>
+  </si>
+  <si>
+    <t>+26969-232</t>
+  </si>
+  <si>
+    <t>+30771-65</t>
+  </si>
+  <si>
+    <t>+17293-220</t>
+  </si>
+  <si>
+    <t>+17301-220</t>
+  </si>
+  <si>
+    <t>+3721-696</t>
+  </si>
+  <si>
+    <t>+187088-77</t>
+  </si>
+  <si>
+    <t>+169-1530</t>
+  </si>
+  <si>
+    <t>+5667-281</t>
+  </si>
+  <si>
+    <t>+2016-705</t>
+  </si>
+  <si>
+    <t>+0035-1583</t>
+  </si>
+  <si>
+    <t>+619-577</t>
+  </si>
+  <si>
+    <t>+1087-1222</t>
+  </si>
+  <si>
+    <t>+26974-232</t>
+  </si>
+  <si>
+    <t>+2445-1369</t>
+  </si>
+  <si>
+    <t>+26979-232</t>
+  </si>
+  <si>
+    <t>+401-1454</t>
+  </si>
+  <si>
+    <t>+26978-232</t>
+  </si>
+  <si>
+    <t>+19923-115</t>
+  </si>
+  <si>
+    <t>+26972-232</t>
+  </si>
+  <si>
+    <t>+242-1524</t>
+  </si>
+  <si>
+    <t>+162-2197</t>
+  </si>
+  <si>
+    <t>+1858-1321</t>
+  </si>
+  <si>
+    <t>+916-1429</t>
+  </si>
+  <si>
+    <t>+1738-1202</t>
+  </si>
+  <si>
+    <t>+1512-886</t>
+  </si>
+  <si>
+    <t>+13083-206</t>
+  </si>
+  <si>
+    <t>+5758-694</t>
+  </si>
+  <si>
+    <t>+187051-77</t>
+  </si>
+  <si>
+    <t>+186995-77</t>
+  </si>
+  <si>
+    <t>+216-1496</t>
+  </si>
+  <si>
+    <t>+187052-77</t>
+  </si>
+  <si>
+    <t>+471-1345</t>
+  </si>
+  <si>
+    <t>186996-77</t>
+  </si>
+  <si>
+    <t>+3694-687</t>
+  </si>
+  <si>
+    <t>+187061-77</t>
+  </si>
+  <si>
+    <t>+442-598</t>
+  </si>
+  <si>
+    <t>+187058-77</t>
+  </si>
+  <si>
+    <t>+187073-77</t>
+  </si>
+  <si>
+    <t>+6396-667</t>
+  </si>
+  <si>
+    <t>+187055-77</t>
+  </si>
+  <si>
+    <t>+12310-645</t>
+  </si>
+  <si>
+    <t>+6830-370</t>
+  </si>
+  <si>
+    <t>+3517-1088</t>
+  </si>
+  <si>
+    <t>+192-2175</t>
+  </si>
+  <si>
+    <t>+239-1506</t>
+  </si>
+  <si>
+    <t>+662-1341</t>
+  </si>
+  <si>
+    <t>+1368-2060</t>
+  </si>
+  <si>
+    <t>+178-1728</t>
+  </si>
+  <si>
+    <t>+45533-147</t>
+  </si>
+  <si>
+    <t>+2258-656</t>
+  </si>
+  <si>
+    <t>+12632-105</t>
+  </si>
+  <si>
+    <t>+1117-578</t>
+  </si>
+  <si>
+    <t>+0042-1106</t>
+  </si>
+  <si>
+    <t>+526-2016</t>
+  </si>
+  <si>
+    <t>+565-1711</t>
+  </si>
+  <si>
+    <t>+3443-340</t>
+  </si>
+  <si>
+    <t>+3542-543</t>
+  </si>
+  <si>
+    <t>+1532-708</t>
+  </si>
+  <si>
+    <t>+179-1545</t>
+  </si>
+  <si>
+    <t>+2051-780</t>
+  </si>
+  <si>
+    <t>+187068-77</t>
+  </si>
+  <si>
+    <t>+2443-741</t>
+  </si>
+  <si>
+    <t>1197-1237</t>
+  </si>
+  <si>
+    <t>+162-1529</t>
+  </si>
+  <si>
+    <t>+750-1480</t>
+  </si>
+  <si>
+    <t>+13949-138</t>
+  </si>
+  <si>
+    <t>+28359-53</t>
+  </si>
+  <si>
+    <t>+19828-459</t>
+  </si>
+  <si>
+    <t>+18368-112</t>
+  </si>
+  <si>
+    <t>+920-1429</t>
+  </si>
+  <si>
+    <t>+983-2098</t>
+  </si>
+  <si>
+    <t>+402-1454</t>
+  </si>
+  <si>
+    <t>+2964-1211</t>
+  </si>
+  <si>
+    <t>+13948-138</t>
+  </si>
+  <si>
+    <t>+0046-1589</t>
+  </si>
+  <si>
+    <t>+1390-947</t>
+  </si>
+  <si>
+    <t>+917-1429</t>
+  </si>
+  <si>
+    <t>+13947-138</t>
+  </si>
+  <si>
+    <t>+499-1564</t>
+  </si>
+  <si>
+    <t>+26968-232</t>
+  </si>
+  <si>
+    <t>+12436-321</t>
+  </si>
+  <si>
+    <t>+10666-443</t>
+  </si>
+  <si>
+    <t>+2496-754</t>
+  </si>
+  <si>
+    <t>+2993-168</t>
+  </si>
+  <si>
+    <t>+2930-484</t>
+  </si>
+  <si>
+    <t>+604-1198</t>
+  </si>
+  <si>
+    <t>+3423-707</t>
+  </si>
+  <si>
+    <t>+3614-695</t>
+  </si>
+  <si>
+    <t>+225-1559</t>
+  </si>
+  <si>
+    <t>+7023-319</t>
+  </si>
+  <si>
+    <t>+1606-1258</t>
+  </si>
+  <si>
+    <t>+8832-233</t>
+  </si>
+  <si>
+    <t>+919-1429</t>
+  </si>
+  <si>
+    <t>+2764-686</t>
+  </si>
+  <si>
+    <t>+195-1523</t>
+  </si>
+  <si>
+    <t>+10670-443</t>
+  </si>
+  <si>
+    <t>+1350-1071</t>
+  </si>
+  <si>
+    <t>+163-1532</t>
+  </si>
+  <si>
+    <t>+1088-828</t>
+  </si>
+  <si>
+    <t>+2260-656</t>
+  </si>
+  <si>
+    <t>+403-1454</t>
+  </si>
+  <si>
+    <t>+3854-377</t>
+  </si>
+  <si>
+    <t>+0021-1592</t>
+  </si>
+  <si>
+    <t>+38195-31</t>
+  </si>
+  <si>
+    <t>+616-2091</t>
+  </si>
+  <si>
+    <t>+4037-768</t>
+  </si>
+  <si>
+    <t>+999-859</t>
+  </si>
+  <si>
+    <t>+406-1454</t>
+  </si>
+  <si>
+    <t>+1979-651</t>
+  </si>
+  <si>
+    <t>+12637-105</t>
+  </si>
+  <si>
+    <t>+6520-664</t>
+  </si>
+  <si>
+    <t>+202-868</t>
+  </si>
+  <si>
+    <t>+4248-414</t>
+  </si>
+  <si>
+    <t>+880-995</t>
+  </si>
+  <si>
+    <t>+203-868</t>
+  </si>
+  <si>
+    <t>+12599-410</t>
+  </si>
+  <si>
+    <t>+4409-632</t>
+  </si>
+  <si>
+    <t>+2587-1244</t>
+  </si>
+  <si>
+    <t>+0086-2179</t>
+  </si>
+  <si>
+    <t>+6520-417</t>
+  </si>
+  <si>
+    <t>+6519-417</t>
+  </si>
+  <si>
+    <t>+399-1454</t>
+  </si>
+  <si>
+    <t>+290-2144</t>
+  </si>
+  <si>
+    <t>193-1523</t>
+  </si>
+  <si>
+    <t>+719-2033</t>
+  </si>
+  <si>
+    <t>+2155-1317</t>
+  </si>
+  <si>
+    <t>+0069-2200</t>
+  </si>
+  <si>
+    <t>+12096-292</t>
+  </si>
+  <si>
+    <t>+3095-790</t>
+  </si>
+  <si>
+    <t>+405-1454</t>
+  </si>
+  <si>
+    <t>+0085-2179</t>
+  </si>
+  <si>
+    <t>+404-1454</t>
+  </si>
+  <si>
+    <t>+12095-292</t>
+  </si>
+  <si>
+    <t>+0049-1707</t>
+  </si>
+  <si>
+    <t>+3088-784</t>
+  </si>
+  <si>
+    <t>+607-1198</t>
   </si>
 </sst>
 </file>
@@ -1643,17 +2135,838 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A164"/>
   <sheetViews>
-    <sheetView topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="A306" sqref="A1:A306"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1663,7 +2976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71368BD7-53C4-4380-8070-6DA79B686E44}">
   <dimension ref="A1:D307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D307"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new script for incomplete shipment data
</commit_message>
<xml_diff>
--- a/Autostockin/stockin49.xlsx
+++ b/Autostockin/stockin49.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Autostockin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898D0E80-1B04-4F50-9EE2-D58EE1767C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67368FEA-A407-4750-AA6C-C54293FD7006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1853">
   <si>
     <t>+7023-319</t>
   </si>
@@ -4940,6 +4940,660 @@
   </si>
   <si>
     <t>+254-1703</t>
+  </si>
+  <si>
+    <t>+1123-890</t>
+  </si>
+  <si>
+    <t>+1122-890</t>
+  </si>
+  <si>
+    <t>320-1531</t>
+  </si>
+  <si>
+    <t>+0038-1750</t>
+  </si>
+  <si>
+    <t>4707-1205</t>
+  </si>
+  <si>
+    <t>+317-817</t>
+  </si>
+  <si>
+    <t>+4516-748</t>
+  </si>
+  <si>
+    <t>+20585-104</t>
+  </si>
+  <si>
+    <t>+759-563</t>
+  </si>
+  <si>
+    <t>+172-1527</t>
+  </si>
+  <si>
+    <t>+188-1517</t>
+  </si>
+  <si>
+    <t>+2294-1089</t>
+  </si>
+  <si>
+    <t>+915-841</t>
+  </si>
+  <si>
+    <t>+2296-1089</t>
+  </si>
+  <si>
+    <t>+1348-1071</t>
+  </si>
+  <si>
+    <t>+1004-2031</t>
+  </si>
+  <si>
+    <t>+814-2097</t>
+  </si>
+  <si>
+    <t>+3695-687</t>
+  </si>
+  <si>
+    <t>+2961-1211</t>
+  </si>
+  <si>
+    <t>+2310-545</t>
+  </si>
+  <si>
+    <t>+317-1531</t>
+  </si>
+  <si>
+    <t>+0076-1542</t>
+  </si>
+  <si>
+    <t>+20598-104</t>
+  </si>
+  <si>
+    <t>+6841-370</t>
+  </si>
+  <si>
+    <t>+198-1528</t>
+  </si>
+  <si>
+    <t>+650-1341</t>
+  </si>
+  <si>
+    <t>+2295-1089</t>
+  </si>
+  <si>
+    <t>+1752-574</t>
+  </si>
+  <si>
+    <t>+707-2076</t>
+  </si>
+  <si>
+    <t>+840-862</t>
+  </si>
+  <si>
+    <t>+979-1248</t>
+  </si>
+  <si>
+    <t>+6569-242</t>
+  </si>
+  <si>
+    <t>+990-859</t>
+  </si>
+  <si>
+    <t>+1118-578</t>
+  </si>
+  <si>
+    <t>+922-1339</t>
+  </si>
+  <si>
+    <t>+9050-374</t>
+  </si>
+  <si>
+    <t>+9049-374</t>
+  </si>
+  <si>
+    <t>+3833-856</t>
+  </si>
+  <si>
+    <t>+9048-374</t>
+  </si>
+  <si>
+    <t>+758-563</t>
+  </si>
+  <si>
+    <t>+3831-856</t>
+  </si>
+  <si>
+    <t>+4619-359</t>
+  </si>
+  <si>
+    <t>+18247-280</t>
+  </si>
+  <si>
+    <t>+1384-887</t>
+  </si>
+  <si>
+    <t>+194-2170</t>
+  </si>
+  <si>
+    <t>+8901-376</t>
+  </si>
+  <si>
+    <t>+6169-640</t>
+  </si>
+  <si>
+    <t>+10538-215</t>
+  </si>
+  <si>
+    <t>+7917-241</t>
+  </si>
+  <si>
+    <t>+2043-706</t>
+  </si>
+  <si>
+    <t>+5311-371</t>
+  </si>
+  <si>
+    <t>+7572-356</t>
+  </si>
+  <si>
+    <t>+315-1525</t>
+  </si>
+  <si>
+    <t>+318-1558</t>
+  </si>
+  <si>
+    <t>+1380-1325</t>
+  </si>
+  <si>
+    <t>+45538-147</t>
+  </si>
+  <si>
+    <t>+2552-759</t>
+  </si>
+  <si>
+    <t>+1523-1310</t>
+  </si>
+  <si>
+    <t>+0031-1579</t>
+  </si>
+  <si>
+    <t>+2763-686</t>
+  </si>
+  <si>
+    <t>+517-1624</t>
+  </si>
+  <si>
+    <t>+1868-940</t>
+  </si>
+  <si>
+    <t>+3352-689</t>
+  </si>
+  <si>
+    <t>+829-2059</t>
+  </si>
+  <si>
+    <t>688-2068</t>
+  </si>
+  <si>
+    <t>+13525-327</t>
+  </si>
+  <si>
+    <t>+8408-290</t>
+  </si>
+  <si>
+    <t>+946-561</t>
+  </si>
+  <si>
+    <t>+938-561</t>
+  </si>
+  <si>
+    <t>+7985-301</t>
+  </si>
+  <si>
+    <t>+3243-869</t>
+  </si>
+  <si>
+    <t>+762-1356</t>
+  </si>
+  <si>
+    <t>+5570-753</t>
+  </si>
+  <si>
+    <t>+647-1108</t>
+  </si>
+  <si>
+    <t>+3242-869</t>
+  </si>
+  <si>
+    <t>+15508-172</t>
+  </si>
+  <si>
+    <t>+6924-500</t>
+  </si>
+  <si>
+    <t>+265-1569</t>
+  </si>
+  <si>
+    <t>+641-1180</t>
+  </si>
+  <si>
+    <t>+2556-773</t>
+  </si>
+  <si>
+    <t>+9797-487</t>
+  </si>
+  <si>
+    <t>+333-1622</t>
+  </si>
+  <si>
+    <t>+874-1438</t>
+  </si>
+  <si>
+    <t>+4957-631</t>
+  </si>
+  <si>
+    <t>+0056-1577</t>
+  </si>
+  <si>
+    <t>12032-150</t>
+  </si>
+  <si>
+    <t>+8576-635</t>
+  </si>
+  <si>
+    <t>+644-1329</t>
+  </si>
+  <si>
+    <t>+8013-498</t>
+  </si>
+  <si>
+    <t>+3832-856</t>
+  </si>
+  <si>
+    <t>+20599-104</t>
+  </si>
+  <si>
+    <t>+9208-84</t>
+  </si>
+  <si>
+    <t>+3366-684</t>
+  </si>
+  <si>
+    <t>837-571</t>
+  </si>
+  <si>
+    <t>+939-1339</t>
+  </si>
+  <si>
+    <t>714-1383</t>
+  </si>
+  <si>
+    <t>+1748-574</t>
+  </si>
+  <si>
+    <t>+2174-1070</t>
+  </si>
+  <si>
+    <t>+2885-389</t>
+  </si>
+  <si>
+    <t>+1147-2002</t>
+  </si>
+  <si>
+    <t>+314-1525</t>
+  </si>
+  <si>
+    <t>+6832-370</t>
+  </si>
+  <si>
+    <t>+45534-147</t>
+  </si>
+  <si>
+    <t>+4168-253</t>
+  </si>
+  <si>
+    <t>+5136-255</t>
+  </si>
+  <si>
+    <t>+1056-874</t>
+  </si>
+  <si>
+    <t>+23152-207</t>
+  </si>
+  <si>
+    <t>+143-1723</t>
+  </si>
+  <si>
+    <t>+140-1723</t>
+  </si>
+  <si>
+    <t>+139-1723</t>
+  </si>
+  <si>
+    <t>+2118-1065</t>
+  </si>
+  <si>
+    <t>+127-1503</t>
+  </si>
+  <si>
+    <t>+147-1740</t>
+  </si>
+  <si>
+    <t>+604-2119</t>
+  </si>
+  <si>
+    <t>+173097-33</t>
+  </si>
+  <si>
+    <t>+194-2181</t>
+  </si>
+  <si>
+    <t>+838-1132</t>
+  </si>
+  <si>
+    <t>+18352-112</t>
+  </si>
+  <si>
+    <t>+5731-797</t>
+  </si>
+  <si>
+    <t>+6466-633</t>
+  </si>
+  <si>
+    <t>+2280-858</t>
+  </si>
+  <si>
+    <t>+413-1505</t>
+  </si>
+  <si>
+    <t>+314-1501</t>
+  </si>
+  <si>
+    <t>+6464-633</t>
+  </si>
+  <si>
+    <t>+1299-544</t>
+  </si>
+  <si>
+    <t>+8800-337</t>
+  </si>
+  <si>
+    <t>+217-829</t>
+  </si>
+  <si>
+    <t>+367-2112</t>
+  </si>
+  <si>
+    <t>+6465-633</t>
+  </si>
+  <si>
+    <t>+430-1616</t>
+  </si>
+  <si>
+    <t>+2612-1048</t>
+  </si>
+  <si>
+    <t>+158-1510</t>
+  </si>
+  <si>
+    <t>+2622-1048</t>
+  </si>
+  <si>
+    <t>+5312-371</t>
+  </si>
+  <si>
+    <t>+2102-412</t>
+  </si>
+  <si>
+    <t>+3491-937</t>
+  </si>
+  <si>
+    <t>+400-1403</t>
+  </si>
+  <si>
+    <t>+0037-1595</t>
+  </si>
+  <si>
+    <t>+210-1518</t>
+  </si>
+  <si>
+    <t>+1321-1213</t>
+  </si>
+  <si>
+    <t>+5282-341</t>
+  </si>
+  <si>
+    <t>+940-1290</t>
+  </si>
+  <si>
+    <t>+900-2048</t>
+  </si>
+  <si>
+    <t>+272-2180</t>
+  </si>
+  <si>
+    <t>+539-2130</t>
+  </si>
+  <si>
+    <t>+802-2007</t>
+  </si>
+  <si>
+    <t>+1005-533</t>
+  </si>
+  <si>
+    <t>+590-1711</t>
+  </si>
+  <si>
+    <t>+1045-2120</t>
+  </si>
+  <si>
+    <t>+895-1170</t>
+  </si>
+  <si>
+    <t>+27058-107</t>
+  </si>
+  <si>
+    <t>+1638-599</t>
+  </si>
+  <si>
+    <t>+850-1167</t>
+  </si>
+  <si>
+    <t>+1120-2055</t>
+  </si>
+  <si>
+    <t>+23900-192</t>
+  </si>
+  <si>
+    <t>+415-1548</t>
+  </si>
+  <si>
+    <t>+4429-618</t>
+  </si>
+  <si>
+    <t>+981-1375</t>
+  </si>
+  <si>
+    <t>+6396-794</t>
+  </si>
+  <si>
+    <t>+866-1193</t>
+  </si>
+  <si>
+    <t>+12552-366</t>
+  </si>
+  <si>
+    <t>762-563</t>
+  </si>
+  <si>
+    <t>+9793-725</t>
+  </si>
+  <si>
+    <t>+4410-273</t>
+  </si>
+  <si>
+    <t>+866-1476</t>
+  </si>
+  <si>
+    <t>+1742-1169</t>
+  </si>
+  <si>
+    <t>+979-2098</t>
+  </si>
+  <si>
+    <t>+119-1720</t>
+  </si>
+  <si>
+    <t>+187064-77</t>
+  </si>
+  <si>
+    <t>+3723-696</t>
+  </si>
+  <si>
+    <t>+173120-33</t>
+  </si>
+  <si>
+    <t>+5308-720</t>
+  </si>
+  <si>
+    <t>+26977-232</t>
+  </si>
+  <si>
+    <t>+7578-356</t>
+  </si>
+  <si>
+    <t>+988-877</t>
+  </si>
+  <si>
+    <t>+35286-222</t>
+  </si>
+  <si>
+    <t>+377-1482</t>
+  </si>
+  <si>
+    <t>+4665-465</t>
+  </si>
+  <si>
+    <t>+3057-1363</t>
+  </si>
+  <si>
+    <t>+288-1507</t>
+  </si>
+  <si>
+    <t>+2776-967</t>
+  </si>
+  <si>
+    <t>+14940-193</t>
+  </si>
+  <si>
+    <t>+1203-875</t>
+  </si>
+  <si>
+    <t>+187097-77</t>
+  </si>
+  <si>
+    <t>+431-1616</t>
+  </si>
+  <si>
+    <t>+1077-1468</t>
+  </si>
+  <si>
+    <t>+187086-77</t>
+  </si>
+  <si>
+    <t>+187047-77</t>
+  </si>
+  <si>
+    <t>+187006-77</t>
+  </si>
+  <si>
+    <t>+187056-77</t>
+  </si>
+  <si>
+    <t>+218-1708</t>
+  </si>
+  <si>
+    <t>+5926-379</t>
+  </si>
+  <si>
+    <t>+806-1380</t>
+  </si>
+  <si>
+    <t>+14842-35</t>
+  </si>
+  <si>
+    <t>+13020-397</t>
+  </si>
+  <si>
+    <t>+12829-191</t>
+  </si>
+  <si>
+    <t>+1248-591</t>
+  </si>
+  <si>
+    <t>+2374-305</t>
+  </si>
+  <si>
+    <t>+2947-1095</t>
+  </si>
+  <si>
+    <t>+10551-215</t>
+  </si>
+  <si>
+    <t>+4496-394</t>
+  </si>
+  <si>
+    <t>+8296-671</t>
+  </si>
+  <si>
+    <t>+540-1195</t>
+  </si>
+  <si>
+    <t>+1194-1342</t>
+  </si>
+  <si>
+    <t>+2565-759</t>
+  </si>
+  <si>
+    <t>+535-1112</t>
+  </si>
+  <si>
+    <t>+2545-776</t>
+  </si>
+  <si>
+    <t>+870-1438</t>
+  </si>
+  <si>
+    <t>+123-1550</t>
+  </si>
+  <si>
+    <t>+35268-222</t>
+  </si>
+  <si>
+    <t>+18249-280</t>
+  </si>
+  <si>
+    <t>+187095-77</t>
+  </si>
+  <si>
+    <t>+35266-222</t>
+  </si>
+  <si>
+    <t>+35271-222</t>
+  </si>
+  <si>
+    <t>+3830-856</t>
+  </si>
+  <si>
+    <t>+1492-1377</t>
+  </si>
+  <si>
+    <t>+1029-1239</t>
+  </si>
+  <si>
+    <t>+187087-77</t>
   </si>
 </sst>
 </file>
@@ -5268,10 +5922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A158"/>
+  <dimension ref="A1:A133"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5281,794 +5935,300 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1477</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1478</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1479</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1480</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1481</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1482</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>1483</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>1484</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1485</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1486</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1487</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1488</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1489</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1490</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1491</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>1492</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>1493</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>1494</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>1495</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1496</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>1497</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>1498</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>1499</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>1500</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>1501</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>1502</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1503</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>1504</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>1505</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>1506</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>1507</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>1508</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>1509</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>1510</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>1511</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>1512</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>1513</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>1514</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>1515</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>1516</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>1517</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>1518</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>1519</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>1520</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>1521</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>1522</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>1523</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1524</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>1525</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>1526</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>1527</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>1528</v>
+        <v>652</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>1529</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>1530</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>1531</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>1532</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>1533</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>1534</v>
+        <v>944</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>1551</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>1607</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>1614</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>1622</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>1628</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>1632</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>1634</v>
-      </c>
-    </row>
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6077,10 +6237,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N380"/>
+  <dimension ref="A1:Q380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N159"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6092,9 +6252,11 @@
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>44828</v>
       </c>
@@ -6137,8 +6299,17 @@
       <c r="N1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2">
+        <v>44838</v>
+      </c>
+      <c r="P1" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>223</v>
       </c>
@@ -6181,8 +6352,14 @@
       <c r="N2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>1635</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>225</v>
       </c>
@@ -6225,8 +6402,14 @@
       <c r="N3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="1" t="s">
+        <v>1636</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>227</v>
       </c>
@@ -6269,8 +6452,14 @@
       <c r="N4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>1637</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>229</v>
       </c>
@@ -6313,8 +6502,14 @@
       <c r="N5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="1" t="s">
+        <v>1638</v>
+      </c>
+      <c r="P5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>231</v>
       </c>
@@ -6357,8 +6552,14 @@
       <c r="N6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="P6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>233</v>
       </c>
@@ -6401,8 +6602,14 @@
       <c r="N7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>235</v>
       </c>
@@ -6445,8 +6652,14 @@
       <c r="N8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>237</v>
       </c>
@@ -6489,8 +6702,14 @@
       <c r="N9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="1" t="s">
+        <v>1642</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>239</v>
       </c>
@@ -6533,8 +6752,14 @@
       <c r="N10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="1" t="s">
+        <v>1643</v>
+      </c>
+      <c r="P10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>241</v>
       </c>
@@ -6577,8 +6802,14 @@
       <c r="N11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="1" t="s">
+        <v>1644</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>243</v>
       </c>
@@ -6621,8 +6852,14 @@
       <c r="N12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>245</v>
       </c>
@@ -6665,8 +6902,14 @@
       <c r="N13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="1" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>247</v>
       </c>
@@ -6709,8 +6952,14 @@
       <c r="N14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="1" t="s">
+        <v>1647</v>
+      </c>
+      <c r="P14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>249</v>
       </c>
@@ -6753,8 +7002,14 @@
       <c r="N15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="1" t="s">
+        <v>1648</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>251</v>
       </c>
@@ -6797,8 +7052,14 @@
       <c r="N16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1" t="s">
+        <v>1649</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>253</v>
       </c>
@@ -6841,8 +7102,14 @@
       <c r="N17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="P17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>255</v>
       </c>
@@ -6885,8 +7152,14 @@
       <c r="N18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="1" t="s">
+        <v>1651</v>
+      </c>
+      <c r="P18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>257</v>
       </c>
@@ -6929,8 +7202,14 @@
       <c r="N19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="P19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>259</v>
       </c>
@@ -6973,8 +7252,14 @@
       <c r="N20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="P20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>261</v>
       </c>
@@ -7017,8 +7302,14 @@
       <c r="N21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="P21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>263</v>
       </c>
@@ -7061,8 +7352,14 @@
       <c r="N22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="P22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>265</v>
       </c>
@@ -7105,8 +7402,14 @@
       <c r="N23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="P23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>267</v>
       </c>
@@ -7149,8 +7452,14 @@
       <c r="N24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="P24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>269</v>
       </c>
@@ -7193,8 +7502,14 @@
       <c r="N25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="1" t="s">
+        <v>1658</v>
+      </c>
+      <c r="P25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>271</v>
       </c>
@@ -7237,8 +7552,14 @@
       <c r="N26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="P26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>273</v>
       </c>
@@ -7281,8 +7602,14 @@
       <c r="N27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="P27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>275</v>
       </c>
@@ -7325,8 +7652,14 @@
       <c r="N28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="P28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>277</v>
       </c>
@@ -7369,8 +7702,14 @@
       <c r="N29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="P29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>279</v>
       </c>
@@ -7413,8 +7752,14 @@
       <c r="N30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="P30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>281</v>
       </c>
@@ -7457,8 +7802,14 @@
       <c r="N31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="P31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>283</v>
       </c>
@@ -7501,8 +7852,14 @@
       <c r="N32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="P32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>285</v>
       </c>
@@ -7545,8 +7902,14 @@
       <c r="N33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="P33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>287</v>
       </c>
@@ -7589,8 +7952,14 @@
       <c r="N34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="P34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>289</v>
       </c>
@@ -7633,8 +8002,14 @@
       <c r="N35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="P35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>291</v>
       </c>
@@ -7677,8 +8052,14 @@
       <c r="N36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="P36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>293</v>
       </c>
@@ -7721,8 +8102,14 @@
       <c r="N37" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="P37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>295</v>
       </c>
@@ -7765,8 +8152,14 @@
       <c r="N38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="P38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>297</v>
       </c>
@@ -7809,8 +8202,14 @@
       <c r="N39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="P39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>299</v>
       </c>
@@ -7853,8 +8252,14 @@
       <c r="N40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="P40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>301</v>
       </c>
@@ -7897,8 +8302,14 @@
       <c r="N41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="1" t="s">
+        <v>1674</v>
+      </c>
+      <c r="P41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>303</v>
       </c>
@@ -7941,8 +8352,14 @@
       <c r="N42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="P42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>305</v>
       </c>
@@ -7985,8 +8402,14 @@
       <c r="N43" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="P43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>307</v>
       </c>
@@ -8029,8 +8452,14 @@
       <c r="N44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="P44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>309</v>
       </c>
@@ -8073,8 +8502,14 @@
       <c r="N45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="P45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>311</v>
       </c>
@@ -8117,8 +8552,14 @@
       <c r="N46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="P46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>313</v>
       </c>
@@ -8161,8 +8602,14 @@
       <c r="N47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="P47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>315</v>
       </c>
@@ -8205,8 +8652,14 @@
       <c r="N48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="P48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -8249,8 +8702,14 @@
       <c r="N49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="P49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>319</v>
       </c>
@@ -8293,8 +8752,14 @@
       <c r="N50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="P50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>321</v>
       </c>
@@ -8337,8 +8802,14 @@
       <c r="N51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="P51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>323</v>
       </c>
@@ -8381,8 +8852,14 @@
       <c r="N52" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="P52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>325</v>
       </c>
@@ -8425,8 +8902,14 @@
       <c r="N53" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="P53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>327</v>
       </c>
@@ -8469,8 +8952,14 @@
       <c r="N54" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="P54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>329</v>
       </c>
@@ -8513,8 +9002,14 @@
       <c r="N55" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="P55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>331</v>
       </c>
@@ -8557,8 +9052,14 @@
       <c r="N56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="P56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>333</v>
       </c>
@@ -8601,8 +9102,14 @@
       <c r="N57" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="P57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>335</v>
       </c>
@@ -8645,8 +9152,14 @@
       <c r="N58" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="P58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>337</v>
       </c>
@@ -8689,8 +9202,14 @@
       <c r="N59" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="P59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>339</v>
       </c>
@@ -8733,8 +9252,14 @@
       <c r="N60" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="P60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>341</v>
       </c>
@@ -8777,8 +9302,14 @@
       <c r="N61" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="P61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>343</v>
       </c>
@@ -8821,8 +9352,14 @@
       <c r="N62" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="P62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>345</v>
       </c>
@@ -8865,8 +9402,14 @@
       <c r="N63" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" s="1" t="s">
+        <v>1696</v>
+      </c>
+      <c r="P63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>347</v>
       </c>
@@ -8909,8 +9452,14 @@
       <c r="N64" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" s="1" t="s">
+        <v>1697</v>
+      </c>
+      <c r="P64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>349</v>
       </c>
@@ -8953,8 +9502,14 @@
       <c r="N65" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="P65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>351</v>
       </c>
@@ -8997,8 +9552,14 @@
       <c r="N66" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" s="1" t="s">
+        <v>1699</v>
+      </c>
+      <c r="P66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>353</v>
       </c>
@@ -9041,8 +9602,14 @@
       <c r="N67" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="P67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>355</v>
       </c>
@@ -9085,8 +9652,14 @@
       <c r="N68" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="P68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>357</v>
       </c>
@@ -9129,8 +9702,14 @@
       <c r="N69" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="P69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>359</v>
       </c>
@@ -9173,8 +9752,14 @@
       <c r="N70" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="P70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>361</v>
       </c>
@@ -9217,8 +9802,14 @@
       <c r="N71" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="P71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>363</v>
       </c>
@@ -9261,8 +9852,14 @@
       <c r="N72" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="P72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>365</v>
       </c>
@@ -9305,8 +9902,14 @@
       <c r="N73" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" s="1" t="s">
+        <v>1706</v>
+      </c>
+      <c r="P73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>367</v>
       </c>
@@ -9349,8 +9952,14 @@
       <c r="N74" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="P74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>369</v>
       </c>
@@ -9393,8 +10002,14 @@
       <c r="N75" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" s="1" t="s">
+        <v>1708</v>
+      </c>
+      <c r="P75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>371</v>
       </c>
@@ -9437,8 +10052,14 @@
       <c r="N76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" s="1" t="s">
+        <v>1709</v>
+      </c>
+      <c r="P76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>373</v>
       </c>
@@ -9481,8 +10102,14 @@
       <c r="N77" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="P77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>375</v>
       </c>
@@ -9525,8 +10152,14 @@
       <c r="N78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="P78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>377</v>
       </c>
@@ -9569,8 +10202,14 @@
       <c r="N79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="P79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>379</v>
       </c>
@@ -9613,8 +10252,14 @@
       <c r="N80" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="P80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>381</v>
       </c>
@@ -9657,8 +10302,14 @@
       <c r="N81" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="P81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>383</v>
       </c>
@@ -9701,8 +10352,14 @@
       <c r="N82" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="P82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>385</v>
       </c>
@@ -9745,8 +10402,14 @@
       <c r="N83" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83" s="1" t="s">
+        <v>1716</v>
+      </c>
+      <c r="P83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>387</v>
       </c>
@@ -9789,8 +10452,14 @@
       <c r="N84" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="P84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>389</v>
       </c>
@@ -9833,8 +10502,14 @@
       <c r="N85" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="P85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>391</v>
       </c>
@@ -9877,8 +10552,14 @@
       <c r="N86" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86" s="1" t="s">
+        <v>1719</v>
+      </c>
+      <c r="P86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>393</v>
       </c>
@@ -9921,8 +10602,14 @@
       <c r="N87" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87" s="1" t="s">
+        <v>1720</v>
+      </c>
+      <c r="P87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>395</v>
       </c>
@@ -9965,8 +10652,14 @@
       <c r="N88" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88" s="1" t="s">
+        <v>1721</v>
+      </c>
+      <c r="P88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>397</v>
       </c>
@@ -10009,8 +10702,14 @@
       <c r="N89" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89" s="1" t="s">
+        <v>1722</v>
+      </c>
+      <c r="P89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>399</v>
       </c>
@@ -10053,8 +10752,14 @@
       <c r="N90" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="P90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>401</v>
       </c>
@@ -10097,8 +10802,14 @@
       <c r="N91" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" s="1" t="s">
+        <v>1724</v>
+      </c>
+      <c r="P91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>403</v>
       </c>
@@ -10141,8 +10852,14 @@
       <c r="N92" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92" s="1" t="s">
+        <v>1725</v>
+      </c>
+      <c r="P92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>405</v>
       </c>
@@ -10185,8 +10902,14 @@
       <c r="N93" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93" s="1" t="s">
+        <v>1726</v>
+      </c>
+      <c r="P93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>407</v>
       </c>
@@ -10229,8 +10952,14 @@
       <c r="N94" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94" s="1" t="s">
+        <v>1727</v>
+      </c>
+      <c r="P94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>409</v>
       </c>
@@ -10273,8 +11002,14 @@
       <c r="N95" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95" s="1" t="s">
+        <v>1728</v>
+      </c>
+      <c r="P95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>411</v>
       </c>
@@ -10317,8 +11052,14 @@
       <c r="N96" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="P96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>413</v>
       </c>
@@ -10361,8 +11102,14 @@
       <c r="N97" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97" s="1" t="s">
+        <v>1730</v>
+      </c>
+      <c r="P97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>415</v>
       </c>
@@ -10405,8 +11152,14 @@
       <c r="N98" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98" s="1" t="s">
+        <v>1731</v>
+      </c>
+      <c r="P98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>417</v>
       </c>
@@ -10449,8 +11202,14 @@
       <c r="N99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99" s="1" t="s">
+        <v>1732</v>
+      </c>
+      <c r="P99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>419</v>
       </c>
@@ -10493,8 +11252,14 @@
       <c r="N100" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100" s="1" t="s">
+        <v>1733</v>
+      </c>
+      <c r="P100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>421</v>
       </c>
@@ -10537,8 +11302,14 @@
       <c r="N101" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101" s="1" t="s">
+        <v>1734</v>
+      </c>
+      <c r="P101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>423</v>
       </c>
@@ -10581,8 +11352,14 @@
       <c r="N102" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102" s="1" t="s">
+        <v>1735</v>
+      </c>
+      <c r="P102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>425</v>
       </c>
@@ -10625,8 +11402,14 @@
       <c r="N103" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103" s="1" t="s">
+        <v>1736</v>
+      </c>
+      <c r="P103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>427</v>
       </c>
@@ -10669,8 +11452,14 @@
       <c r="N104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104" s="1" t="s">
+        <v>1737</v>
+      </c>
+      <c r="P104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>429</v>
       </c>
@@ -10713,8 +11502,14 @@
       <c r="N105" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="P105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>431</v>
       </c>
@@ -10757,8 +11552,14 @@
       <c r="N106" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106" s="1" t="s">
+        <v>1739</v>
+      </c>
+      <c r="P106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>433</v>
       </c>
@@ -10801,8 +11602,14 @@
       <c r="N107" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107" s="1" t="s">
+        <v>1740</v>
+      </c>
+      <c r="P107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>435</v>
       </c>
@@ -10845,8 +11652,14 @@
       <c r="N108" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108" s="1" t="s">
+        <v>1741</v>
+      </c>
+      <c r="P108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>437</v>
       </c>
@@ -10889,8 +11702,14 @@
       <c r="N109" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109" s="1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="P109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>439</v>
       </c>
@@ -10933,8 +11752,14 @@
       <c r="N110" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="P110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>441</v>
       </c>
@@ -10977,8 +11802,14 @@
       <c r="N111" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O111" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="P111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>443</v>
       </c>
@@ -11021,8 +11852,14 @@
       <c r="N112" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="P112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>445</v>
       </c>
@@ -11065,8 +11902,14 @@
       <c r="N113" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="P113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>447</v>
       </c>
@@ -11109,8 +11952,14 @@
       <c r="N114" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="P114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>449</v>
       </c>
@@ -11153,8 +12002,14 @@
       <c r="N115" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="P115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>451</v>
       </c>
@@ -11197,8 +12052,14 @@
       <c r="N116" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="P116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>453</v>
       </c>
@@ -11241,8 +12102,14 @@
       <c r="N117" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117" s="1" t="s">
+        <v>1750</v>
+      </c>
+      <c r="P117" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>455</v>
       </c>
@@ -11285,8 +12152,14 @@
       <c r="N118" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="P118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>457</v>
       </c>
@@ -11329,8 +12202,14 @@
       <c r="N119" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="P119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>459</v>
       </c>
@@ -11373,8 +12252,14 @@
       <c r="N120" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="P120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>461</v>
       </c>
@@ -11417,8 +12302,14 @@
       <c r="N121" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="P121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>463</v>
       </c>
@@ -11461,8 +12352,14 @@
       <c r="N122" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="P122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>465</v>
       </c>
@@ -11505,8 +12402,14 @@
       <c r="N123" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="P123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>467</v>
       </c>
@@ -11549,8 +12452,14 @@
       <c r="N124" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124" s="1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="P124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C125" s="1" t="s">
         <v>469</v>
       </c>
@@ -11587,8 +12496,14 @@
       <c r="N125" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="P125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C126" s="1" t="s">
         <v>470</v>
       </c>
@@ -11625,8 +12540,14 @@
       <c r="N126" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O126" s="1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="P126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C127" s="1" t="s">
         <v>471</v>
       </c>
@@ -11663,8 +12584,14 @@
       <c r="N127" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O127" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="P127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C128" s="1" t="s">
         <v>472</v>
       </c>
@@ -11701,8 +12628,14 @@
       <c r="N128" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O128" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="P128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
         <v>473</v>
       </c>
@@ -11739,8 +12672,14 @@
       <c r="N129" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O129" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="P129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C130" s="1" t="s">
         <v>474</v>
       </c>
@@ -11777,8 +12716,14 @@
       <c r="N130" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="131" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O130" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="P130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C131" s="1" t="s">
         <v>475</v>
       </c>
@@ -11815,8 +12760,14 @@
       <c r="N131" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="132" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O131" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="P131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C132" s="1" t="s">
         <v>476</v>
       </c>
@@ -11853,8 +12804,14 @@
       <c r="N132" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O132" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="P132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
         <v>477</v>
       </c>
@@ -11891,8 +12848,14 @@
       <c r="N133" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O133" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="P133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C134" s="1" t="s">
         <v>478</v>
       </c>
@@ -11929,8 +12892,14 @@
       <c r="N134" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O134" s="1" t="s">
+        <v>1767</v>
+      </c>
+      <c r="P134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C135" s="1" t="s">
         <v>479</v>
       </c>
@@ -11967,8 +12936,14 @@
       <c r="N135" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="136" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O135" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="P135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C136" s="1" t="s">
         <v>480</v>
       </c>
@@ -12005,8 +12980,14 @@
       <c r="N136" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O136" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="P136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C137" s="1" t="s">
         <v>481</v>
       </c>
@@ -12043,8 +13024,14 @@
       <c r="N137" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="138" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O137" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="P137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C138" s="1" t="s">
         <v>482</v>
       </c>
@@ -12081,8 +13068,14 @@
       <c r="N138" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="139" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O138" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="P138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
         <v>483</v>
       </c>
@@ -12119,8 +13112,14 @@
       <c r="N139" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="140" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O139" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="P139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C140" s="1" t="s">
         <v>484</v>
       </c>
@@ -12157,8 +13156,14 @@
       <c r="N140" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="141" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O140" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="P140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C141" s="1" t="s">
         <v>485</v>
       </c>
@@ -12195,8 +13200,14 @@
       <c r="N141" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O141" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="P141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C142" s="1" t="s">
         <v>486</v>
       </c>
@@ -12233,8 +13244,14 @@
       <c r="N142" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="143" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O142" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="P142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C143" s="1" t="s">
         <v>487</v>
       </c>
@@ -12271,8 +13288,14 @@
       <c r="N143" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="144" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O143" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="P143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C144" s="1" t="s">
         <v>488</v>
       </c>
@@ -12309,8 +13332,14 @@
       <c r="N144" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="145" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O144" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="P144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
         <v>489</v>
       </c>
@@ -12347,8 +13376,14 @@
       <c r="N145" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="146" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O145" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="P145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C146" s="1" t="s">
         <v>490</v>
       </c>
@@ -12385,8 +13420,14 @@
       <c r="N146" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="147" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O146" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="P146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
         <v>491</v>
       </c>
@@ -12423,8 +13464,14 @@
       <c r="N147" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O147" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="P147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C148" s="1" t="s">
         <v>492</v>
       </c>
@@ -12461,8 +13508,14 @@
       <c r="N148" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="149" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O148" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="P148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
         <v>493</v>
       </c>
@@ -12499,8 +13552,14 @@
       <c r="N149" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="150" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O149" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="P149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C150" s="1" t="s">
         <v>494</v>
       </c>
@@ -12537,8 +13596,14 @@
       <c r="N150" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="151" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O150" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="P150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
         <v>495</v>
       </c>
@@ -12575,8 +13640,14 @@
       <c r="N151" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="152" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O151" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="P151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C152" s="1" t="s">
         <v>496</v>
       </c>
@@ -12613,8 +13684,14 @@
       <c r="N152" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="153" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O152" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="P152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C153" s="1" t="s">
         <v>497</v>
       </c>
@@ -12651,8 +13728,14 @@
       <c r="N153" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O153" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="P153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C154" s="1" t="s">
         <v>498</v>
       </c>
@@ -12689,8 +13772,14 @@
       <c r="N154" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="155" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O154" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="P154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
         <v>499</v>
       </c>
@@ -12727,8 +13816,14 @@
       <c r="N155" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="156" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O155" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="P155" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C156" s="1" t="s">
         <v>500</v>
       </c>
@@ -12765,8 +13860,14 @@
       <c r="N156" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O156" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="P156" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C157" s="1" t="s">
         <v>501</v>
       </c>
@@ -12803,8 +13904,14 @@
       <c r="N157" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="158" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O157" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="P157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C158" s="1" t="s">
         <v>502</v>
       </c>
@@ -12841,8 +13948,14 @@
       <c r="N158" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O158" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="P158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
         <v>503</v>
       </c>
@@ -12879,8 +13992,14 @@
       <c r="N159" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="160" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O159" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="P159" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C160" s="1" t="s">
         <v>504</v>
       </c>
@@ -12911,8 +14030,14 @@
       <c r="L160" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O160" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="P160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C161" s="1" t="s">
         <v>505</v>
       </c>
@@ -12943,8 +14068,14 @@
       <c r="L161" t="s">
         <v>1476</v>
       </c>
-    </row>
-    <row r="162" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O161" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="P161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C162" s="1" t="s">
         <v>506</v>
       </c>
@@ -12975,8 +14106,14 @@
       <c r="L162" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="163" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O162" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="P162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C163" s="1" t="s">
         <v>507</v>
       </c>
@@ -13007,8 +14144,14 @@
       <c r="L163" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="164" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O163" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="P163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C164" s="1" t="s">
         <v>508</v>
       </c>
@@ -13039,8 +14182,14 @@
       <c r="L164" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="165" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O164" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="P164" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
         <v>509</v>
       </c>
@@ -13065,8 +14214,14 @@
       <c r="J165" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="166" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="O165" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="P165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C166" s="1" t="s">
         <v>510</v>
       </c>
@@ -13092,7 +14247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
         <v>511</v>
       </c>
@@ -13118,7 +14273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C168" s="1" t="s">
         <v>512</v>
       </c>
@@ -13138,7 +14293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
         <v>513</v>
       </c>
@@ -13158,7 +14313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C170" s="1" t="s">
         <v>514</v>
       </c>
@@ -13178,7 +14333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C171" s="1" t="s">
         <v>515</v>
       </c>
@@ -13198,7 +14353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C172" s="1" t="s">
         <v>516</v>
       </c>
@@ -13218,7 +14373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
         <v>517</v>
       </c>
@@ -13238,7 +14393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C174" s="1" t="s">
         <v>518</v>
       </c>
@@ -13258,7 +14413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C175" s="1" t="s">
         <v>519</v>
       </c>
@@ -13278,7 +14433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C176" s="1" t="s">
         <v>520</v>
       </c>

</xml_diff>